<commit_message>
Code clean up + a few comments
</commit_message>
<xml_diff>
--- a/NLP/main/output/quotes.xlsx
+++ b/NLP/main/output/quotes.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,62 +441,52 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>quote_id</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>quote_id</t>
+          <t>quote</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>quote</t>
+          <t>quote_index</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>quote_index</t>
+          <t>speaker</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>speaker</t>
+          <t>speaker_index</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>speaker_index</t>
+          <t>verb</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>verb</t>
+          <t>verb_index</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>verb_index</t>
+          <t>quote_token_count</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>quote_token_count</t>
+          <t>quote_type</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>quote_type</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
           <t>is_floating_quote</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>text_spacy</t>
         </is>
       </c>
     </row>
@@ -508,71 +498,49 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>"We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States."</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>"We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States."</t>
+          <t>(1052, 1238)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>(1052, 1238)</t>
+          <t>Grygiel</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Grygiel</t>
+          <t>(1239, 1246)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>(1239, 1246)</t>
+          <t>said</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>said</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
           <t>(1247, 1251)</t>
         </is>
       </c>
-      <c r="J2" t="n">
+      <c r="I2" t="n">
         <v>38</v>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Heuristic</t>
         </is>
       </c>
-      <c r="L2" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
-        </is>
+      <c r="K2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -583,67 +551,45 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>"Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States."</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>"Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States."</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
           <t>(1492, 1691)</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>(0, 0)</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>(0, 0)</t>
+          <t>caused</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>caused</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
           <t>(1705, 1711)</t>
         </is>
       </c>
-      <c r="J3" t="n">
+      <c r="I3" t="n">
         <v>39</v>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>Heuristic</t>
         </is>
       </c>
-      <c r="L3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
-        </is>
+      <c r="K3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -654,71 +600,49 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>that Trump wouldn't be able to post for 24 hours following two violations of its policies</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>that Trump wouldn't be able to post for 24 hours following two violations of its policies</t>
+          <t>(84, 173)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>(84, 173)</t>
+          <t>Facebook and Instagram, which Facebook owns,</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Facebook and Instagram, which Facebook owns,</t>
+          <t>(0, 44)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>(0, 44)</t>
+          <t>announcing</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>announcing</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
           <t>(73, 83)</t>
         </is>
       </c>
-      <c r="J4" t="n">
+      <c r="I4" t="n">
         <v>17</v>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>S V C</t>
         </is>
       </c>
-      <c r="L4" t="b">
-        <v>0</v>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
-        </is>
+      <c r="K4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -729,71 +653,49 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events</t>
+          <t>(302, 489)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>(302, 489)</t>
+          <t>experts</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>experts</t>
+          <t>(288, 295)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>(288, 295)</t>
+          <t>noted</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>noted</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
           <t>(296, 301)</t>
         </is>
       </c>
-      <c r="J5" t="n">
+      <c r="I5" t="n">
         <v>26</v>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>S V C</t>
         </is>
       </c>
-      <c r="L5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
-        </is>
+      <c r="K5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -804,71 +706,49 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction</t>
+          <t>(592, 813)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>(592, 813)</t>
+          <t>Jennifer Grygiel, a Syracuse University communications professor and an expert on social media,</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Jennifer Grygiel, a Syracuse University communications professor and an expert on social media,</t>
+          <t>(491, 586)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>(491, 586)</t>
+          <t>said</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>said</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
           <t>(587, 591)</t>
         </is>
       </c>
-      <c r="J6" t="n">
+      <c r="I6" t="n">
         <v>38</v>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>S V C</t>
         </is>
       </c>
-      <c r="L6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
-        </is>
+      <c r="K6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -879,72 +759,50 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
         <is>
           <t xml:space="preserve">
  "This is what happens</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>(1012, 1035)</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>(1012, 1035)</t>
+          <t>Grygiel</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Grygiel</t>
+          <t>(1038, 1045)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>(1038, 1045)</t>
+          <t>said</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>said</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
           <t>(1046, 1050)</t>
         </is>
       </c>
-      <c r="J7" t="n">
+      <c r="I7" t="n">
         <v>6</v>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>C S V</t>
         </is>
       </c>
-      <c r="L7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
-        </is>
+      <c r="K7" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -955,71 +813,49 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>They're creeping along towards firmer action</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>They're creeping along towards firmer action</t>
+          <t>(1352, 1396)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>(1352, 1396)</t>
+          <t>Grygiel</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Grygiel</t>
+          <t>(1399, 1406)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>(1399, 1406)</t>
+          <t>said</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>said</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
           <t>(1407, 1411)</t>
         </is>
       </c>
-      <c r="J8" t="n">
+      <c r="I8" t="n">
         <v>7</v>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>Q C Q S V</t>
         </is>
       </c>
-      <c r="L8" t="b">
-        <v>0</v>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
-        </is>
+      <c r="K8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1030,71 +866,49 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
+          <t>7</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence</t>
+          <t>(2362, 2467)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>(2362, 2467)</t>
+          <t>Guy Rosen, Facebook's vice-president of integrity,</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Guy Rosen, Facebook's vice-president of integrity,</t>
+          <t>(2285, 2335)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>(2285, 2335)</t>
+          <t>said</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>said</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
           <t>(2336, 2340)</t>
         </is>
       </c>
-      <c r="J9" t="n">
+      <c r="I9" t="n">
         <v>18</v>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>S V C</t>
         </is>
       </c>
-      <c r="L9" t="b">
-        <v>0</v>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
-        </is>
+      <c r="K9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1105,71 +919,49 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video</t>
+          <t>(2471, 2594)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>(2471, 2594)</t>
+          <t>Rosen</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Rosen</t>
+          <t>(2597, 2602)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>(2597, 2602)</t>
+          <t>said</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>said</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
           <t>(2603, 2607)</t>
         </is>
       </c>
-      <c r="J10" t="n">
+      <c r="I10" t="n">
         <v>19</v>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>Q C Q S V</t>
         </is>
       </c>
-      <c r="L10" t="b">
-        <v>0</v>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
-        </is>
+      <c r="K10" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1180,71 +972,49 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>I know your pain</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>I know your pain</t>
+          <t>(2803, 2819)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>(2803, 2819)</t>
+          <t>his video</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>his video</t>
+          <t>(2784, 2793)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>(2784, 2793)</t>
+          <t>saying</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>saying</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
           <t>(2794, 2800)</t>
         </is>
       </c>
-      <c r="J11" t="n">
+      <c r="I11" t="n">
         <v>4</v>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>S V C</t>
         </is>
       </c>
-      <c r="L11" t="b">
-        <v>0</v>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
-        </is>
+      <c r="K11" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1255,71 +1025,49 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>We can't play into the hands of these people</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>We can't play into the hands of these people</t>
+          <t>(2963, 3007)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>(2963, 3007)</t>
+          <t>Trump</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Trump</t>
+          <t>(2940, 2945)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>(2940, 2945)</t>
+          <t>say</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>say</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
           <t>(2957, 2960)</t>
         </is>
       </c>
-      <c r="J12" t="n">
+      <c r="I12" t="n">
         <v>10</v>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>S V C</t>
         </is>
       </c>
-      <c r="L12" t="b">
-        <v>0</v>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>Facebook and Instagram, which Facebook owns, followed up in the evening, announcing that Trump wouldn't be able to post for 24 hours following two violations of its policies. The White House did not immediately offer a response to the actions. While some cheered the platforms' response, experts noted that these actions follow years of hemming and hawing regarding Trump and his supporters spreading dangerous misinformation and encouraging violence that contributed to Wednesday's events. Jennifer Grygiel, a Syracuse University communications professor and an expert on social media, said what happened in Washington, D.C., on Wednesday is a direct result of Trump's use of social media to spread propaganda and disinformation, and that the platforms should bear some responsibility for their previous inaction. Police secure U.S. Capitol after pro-Trump rioters cause bedlam at heart of U.S. government.
- Senate, House resoundingly reject 1st challenge to Biden win hours after angry mob storms U.S. Capitol.
- "This is what happens," Grygiel said. "We didn't just see a breach at the Capitol. Social media platforms have been breached by the president repeatedly. This is disinformation. This was a coup attempt in the United States." Grygiel said the platform's decision to remove the video — and Twitter's suspension — are too little, too late. "They're creeping along towards firmer action," Grygiel said, calling Trump "Exhibit A" for the need for greater regulation of social media. "Social media is complicit in this because he has repeatedly used social media to incite violence. It's a culmination of years of propaganda and abuse of media by the president of the United States." An explosion caused by a police munition is seen while supporters of U.S. President Donald Trump gather in front of the U.S. Capitol in Washington on Jan. 6. Congress had been meeting to ratify president-elect Joe Biden's 306-232 electoral college win over Trump. (Leah Millis/Reuters).
- Show next image (2 of 25).
- Hide caption.
- Toggle Fullscreen1 of 25.
- Trump posted the video more than two hours after protesters entered the Capitol, interrupting lawmakers meeting in a joint session to confirm the electoral college results and president-elect Joe Biden's victory. Too little, too late? Guy Rosen, Facebook's vice-president of integrity, said on Twitter Wednesday that the video was removed because it "contributes to rather than diminishes the risk of ongoing violence." "This is an emergency situation and we are taking appropriate emergency measures, including removing President Trump's video," Rosen said. Twitter initially left the video up but blocked people from being able to retweet it or comment on it. Only later in the day did the platform delete it entirely. Trump opened his video saying, "I know your pain. I know your hurt. But you have to go home now." After repeating false claims about voter fraud affecting the election, Trump went on to say: "We can't play into the hands of these people. We have to have peace. So go home. We love you. You're very special."</t>
-        </is>
+      <c r="K12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1330,57 +1078,41 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>(CBC News).
- Republican lawmakers and previous administration officials had begged Trump to give a statement to his supporters to quell the violence. He posted his video as authorities struggled to take control of a chaotic situation at the Capitol that led to the evacuation of lawmakers and the death of at least one person. Lawmakers, world leaders condemn chaos at the U.S. Capitol while some call for Trump's removal.
- Trudeau says Canadians 'deeply disturbed' by violence in Washington D.C.
- Trump has harnessed social media — especially Twitter — as a potent tool for spreading misinformation about the election. Wednesday's riot only increased calls to ban Trump from the platform. "The President has promoted sedition and incited violence," said Jonathan Greenblatt, chief executive officer of the Anti-Defamation League, in a statement. "More than anything, what is happening right now at the Capitol is a direct result of the fear and disinformation that has been spewed consistently from the Oval Office." In a statement Thursday morning, Trump said there would be an "orderly transition on January 20th" and acknowledged defeat in the election for the first time. His aides posted the statement on Twitter because his account remained suspended.</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>"More than anything, what is happening right now at the Capitol is a direct result of the fear and disinformation that has been spewed consistently from the Oval Office."</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>"More than anything, what is happening right now at the Capitol is a direct result of the fear and disinformation that has been spewed consistently from the Oval Office."</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
           <t>(847, 1017)</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr">
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
         <is>
           <t>(0, 0)</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr">
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
         <is>
           <t>(0, 0)</t>
         </is>
       </c>
-      <c r="J13" t="n">
+      <c r="I13" t="n">
         <v>33</v>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>Heuristic</t>
         </is>
       </c>
-      <c r="L13" t="b">
-        <v>0</v>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>(CBC News).
- Republican lawmakers and previous administration officials had begged Trump to give a statement to his supporters to quell the violence. He posted his video as authorities struggled to take control of a chaotic situation at the Capitol that led to the evacuation of lawmakers and the death of at least one person. Lawmakers, world leaders condemn chaos at the U.S. Capitol while some call for Trump's removal.
- Trudeau says Canadians 'deeply disturbed' by violence in Washington D.C.
- Trump has harnessed social media — especially Twitter — as a potent tool for spreading misinformation about the election. Wednesday's riot only increased calls to ban Trump from the platform. "The President has promoted sedition and incited violence," said Jonathan Greenblatt, chief executive officer of the Anti-Defamation League, in a statement. "More than anything, what is happening right now at the Capitol is a direct result of the fear and disinformation that has been spewed consistently from the Oval Office." In a statement Thursday morning, Trump said there would be an "orderly transition on January 20th" and acknowledged defeat in the election for the first time. His aides posted the statement on Twitter because his account remained suspended.</t>
-        </is>
+      <c r="K13" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1391,65 +1123,49 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>(CBC News).
- Republican lawmakers and previous administration officials had begged Trump to give a statement to his supporters to quell the violence. He posted his video as authorities struggled to take control of a chaotic situation at the Capitol that led to the evacuation of lawmakers and the death of at least one person. Lawmakers, world leaders condemn chaos at the U.S. Capitol while some call for Trump's removal.
- Trudeau says Canadians 'deeply disturbed' by violence in Washington D.C.
- Trump has harnessed social media — especially Twitter — as a potent tool for spreading misinformation about the election. Wednesday's riot only increased calls to ban Trump from the platform. "The President has promoted sedition and incited violence," said Jonathan Greenblatt, chief executive officer of the Anti-Defamation League, in a statement. "More than anything, what is happening right now at the Capitol is a direct result of the fear and disinformation that has been spewed consistently from the Oval Office." In a statement Thursday morning, Trump said there would be an "orderly transition on January 20th" and acknowledged defeat in the election for the first time. His aides posted the statement on Twitter because his account remained suspended.</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Canadians 'deeply disturbed' by violence in Washington D.C.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Canadians 'deeply disturbed' by violence in Washington D.C.</t>
+          <t>(437, 496)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>(437, 496)</t>
+          <t>Trudeau</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Trudeau</t>
+          <t>(424, 431)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>(424, 431)</t>
+          <t>says</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>says</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
           <t>(432, 436)</t>
         </is>
       </c>
-      <c r="J14" t="n">
+      <c r="I14" t="n">
         <v>10</v>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>S V C</t>
         </is>
       </c>
-      <c r="L14" t="b">
-        <v>0</v>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>(CBC News).
- Republican lawmakers and previous administration officials had begged Trump to give a statement to his supporters to quell the violence. He posted his video as authorities struggled to take control of a chaotic situation at the Capitol that led to the evacuation of lawmakers and the death of at least one person. Lawmakers, world leaders condemn chaos at the U.S. Capitol while some call for Trump's removal.
- Trudeau says Canadians 'deeply disturbed' by violence in Washington D.C.
- Trump has harnessed social media — especially Twitter — as a potent tool for spreading misinformation about the election. Wednesday's riot only increased calls to ban Trump from the platform. "The President has promoted sedition and incited violence," said Jonathan Greenblatt, chief executive officer of the Anti-Defamation League, in a statement. "More than anything, what is happening right now at the Capitol is a direct result of the fear and disinformation that has been spewed consistently from the Oval Office." In a statement Thursday morning, Trump said there would be an "orderly transition on January 20th" and acknowledged defeat in the election for the first time. His aides posted the statement on Twitter because his account remained suspended.</t>
-        </is>
+      <c r="K14" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1460,66 +1176,50 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>(CBC News).
- Republican lawmakers and previous administration officials had begged Trump to give a statement to his supporters to quell the violence. He posted his video as authorities struggled to take control of a chaotic situation at the Capitol that led to the evacuation of lawmakers and the death of at least one person. Lawmakers, world leaders condemn chaos at the U.S. Capitol while some call for Trump's removal.
- Trudeau says Canadians 'deeply disturbed' by violence in Washington D.C.
- Trump has harnessed social media — especially Twitter — as a potent tool for spreading misinformation about the election. Wednesday's riot only increased calls to ban Trump from the platform. "The President has promoted sedition and incited violence," said Jonathan Greenblatt, chief executive officer of the Anti-Defamation League, in a statement. "More than anything, what is happening right now at the Capitol is a direct result of the fear and disinformation that has been spewed consistently from the Oval Office." In a statement Thursday morning, Trump said there would be an "orderly transition on January 20th" and acknowledged defeat in the election for the first time. His aides posted the statement on Twitter because his account remained suspended.</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
         <is>
           <t xml:space="preserve">
  Trump has harnessed social media — especially Twitter — as a potent tool for spreading misinformation about the election</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>(496, 618)</t>
+        </is>
+      </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>(496, 618)</t>
+          <t>Trudeau</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Trudeau</t>
+          <t>(424, 431)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>(424, 431)</t>
+          <t>says</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>says</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
           <t>(432, 436)</t>
         </is>
       </c>
-      <c r="J15" t="n">
+      <c r="I15" t="n">
         <v>20</v>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>S V C</t>
         </is>
       </c>
-      <c r="L15" t="b">
-        <v>0</v>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>(CBC News).
- Republican lawmakers and previous administration officials had begged Trump to give a statement to his supporters to quell the violence. He posted his video as authorities struggled to take control of a chaotic situation at the Capitol that led to the evacuation of lawmakers and the death of at least one person. Lawmakers, world leaders condemn chaos at the U.S. Capitol while some call for Trump's removal.
- Trudeau says Canadians 'deeply disturbed' by violence in Washington D.C.
- Trump has harnessed social media — especially Twitter — as a potent tool for spreading misinformation about the election. Wednesday's riot only increased calls to ban Trump from the platform. "The President has promoted sedition and incited violence," said Jonathan Greenblatt, chief executive officer of the Anti-Defamation League, in a statement. "More than anything, what is happening right now at the Capitol is a direct result of the fear and disinformation that has been spewed consistently from the Oval Office." In a statement Thursday morning, Trump said there would be an "orderly transition on January 20th" and acknowledged defeat in the election for the first time. His aides posted the statement on Twitter because his account remained suspended.</t>
-        </is>
+      <c r="K15" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1530,65 +1230,49 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>(CBC News).
- Republican lawmakers and previous administration officials had begged Trump to give a statement to his supporters to quell the violence. He posted his video as authorities struggled to take control of a chaotic situation at the Capitol that led to the evacuation of lawmakers and the death of at least one person. Lawmakers, world leaders condemn chaos at the U.S. Capitol while some call for Trump's removal.
- Trudeau says Canadians 'deeply disturbed' by violence in Washington D.C.
- Trump has harnessed social media — especially Twitter — as a potent tool for spreading misinformation about the election. Wednesday's riot only increased calls to ban Trump from the platform. "The President has promoted sedition and incited violence," said Jonathan Greenblatt, chief executive officer of the Anti-Defamation League, in a statement. "More than anything, what is happening right now at the Capitol is a direct result of the fear and disinformation that has been spewed consistently from the Oval Office." In a statement Thursday morning, Trump said there would be an "orderly transition on January 20th" and acknowledged defeat in the election for the first time. His aides posted the statement on Twitter because his account remained suspended.</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>"The President has promoted sedition and incited violence</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>"The President has promoted sedition and incited violence</t>
+          <t>(690, 747)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>(690, 747)</t>
+          <t>Jonathan Greenblatt, chief executive officer of the Anti-Defamation League,</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Jonathan Greenblatt, chief executive officer of the Anti-Defamation League,</t>
+          <t>(755, 830)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>(755, 830)</t>
+          <t>said</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>said</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
           <t>(750, 754)</t>
         </is>
       </c>
-      <c r="J16" t="n">
+      <c r="I16" t="n">
         <v>9</v>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>Q C Q V S</t>
         </is>
       </c>
-      <c r="L16" t="b">
-        <v>0</v>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>(CBC News).
- Republican lawmakers and previous administration officials had begged Trump to give a statement to his supporters to quell the violence. He posted his video as authorities struggled to take control of a chaotic situation at the Capitol that led to the evacuation of lawmakers and the death of at least one person. Lawmakers, world leaders condemn chaos at the U.S. Capitol while some call for Trump's removal.
- Trudeau says Canadians 'deeply disturbed' by violence in Washington D.C.
- Trump has harnessed social media — especially Twitter — as a potent tool for spreading misinformation about the election. Wednesday's riot only increased calls to ban Trump from the platform. "The President has promoted sedition and incited violence," said Jonathan Greenblatt, chief executive officer of the Anti-Defamation League, in a statement. "More than anything, what is happening right now at the Capitol is a direct result of the fear and disinformation that has been spewed consistently from the Oval Office." In a statement Thursday morning, Trump said there would be an "orderly transition on January 20th" and acknowledged defeat in the election for the first time. His aides posted the statement on Twitter because his account remained suspended.</t>
-        </is>
+      <c r="K16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1599,65 +1283,49 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>(CBC News).
- Republican lawmakers and previous administration officials had begged Trump to give a statement to his supporters to quell the violence. He posted his video as authorities struggled to take control of a chaotic situation at the Capitol that led to the evacuation of lawmakers and the death of at least one person. Lawmakers, world leaders condemn chaos at the U.S. Capitol while some call for Trump's removal.
- Trudeau says Canadians 'deeply disturbed' by violence in Washington D.C.
- Trump has harnessed social media — especially Twitter — as a potent tool for spreading misinformation about the election. Wednesday's riot only increased calls to ban Trump from the platform. "The President has promoted sedition and incited violence," said Jonathan Greenblatt, chief executive officer of the Anti-Defamation League, in a statement. "More than anything, what is happening right now at the Capitol is a direct result of the fear and disinformation that has been spewed consistently from the Oval Office." In a statement Thursday morning, Trump said there would be an "orderly transition on January 20th" and acknowledged defeat in the election for the first time. His aides posted the statement on Twitter because his account remained suspended.</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>there would be an "orderly transition on January 20th" and acknowledged defeat in the election for the first time</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>there would be an "orderly transition on January 20th" and acknowledged defeat in the election for the first time</t>
+          <t>(1062, 1175)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>(1062, 1175)</t>
+          <t>Trump</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Trump</t>
+          <t>(1051, 1056)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>(1051, 1056)</t>
+          <t>said</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>said</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
           <t>(1057, 1061)</t>
         </is>
       </c>
-      <c r="J17" t="n">
+      <c r="I17" t="n">
         <v>21</v>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>S V C</t>
         </is>
       </c>
-      <c r="L17" t="b">
-        <v>0</v>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>(CBC News).
- Republican lawmakers and previous administration officials had begged Trump to give a statement to his supporters to quell the violence. He posted his video as authorities struggled to take control of a chaotic situation at the Capitol that led to the evacuation of lawmakers and the death of at least one person. Lawmakers, world leaders condemn chaos at the U.S. Capitol while some call for Trump's removal.
- Trudeau says Canadians 'deeply disturbed' by violence in Washington D.C.
- Trump has harnessed social media — especially Twitter — as a potent tool for spreading misinformation about the election. Wednesday's riot only increased calls to ban Trump from the platform. "The President has promoted sedition and incited violence," said Jonathan Greenblatt, chief executive officer of the Anti-Defamation League, in a statement. "More than anything, what is happening right now at the Capitol is a direct result of the fear and disinformation that has been spewed consistently from the Oval Office." In a statement Thursday morning, Trump said there would be an "orderly transition on January 20th" and acknowledged defeat in the election for the first time. His aides posted the statement on Twitter because his account remained suspended.</t>
-        </is>
+      <c r="K17" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1668,59 +1336,49 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Federated States of Micronesia President David Panuelo warned the deal could stoke geopolitical tensions and undermine the sovereignty of the Pacific, while Samoa's Prime Minister, Fiame Naomi Mata'afa, suggested the process had been rushed. Pacific expert Anna Powles from Massey University told the ABC "very little" was currently known about the meeting but it seemed to be part of China's broader attempts to sideline the PIF. "It appears to be an attempt to deliberately disrupt existing regional mechanisms which China is not a part of," she said.</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>the deal could stoke geopolitical tensions and undermine the sovereignty of the Pacific</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>the deal could stoke geopolitical tensions and undermine the sovereignty of the Pacific</t>
+          <t>(62, 149)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>(62, 149)</t>
+          <t>Federated States of Micronesia President David Panuelo</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Federated States of Micronesia President David Panuelo</t>
+          <t>(0, 54)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>(0, 54)</t>
+          <t>warned</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>warned</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
           <t>(55, 61)</t>
         </is>
       </c>
-      <c r="J18" t="n">
+      <c r="I18" t="n">
         <v>13</v>
       </c>
-      <c r="K18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>S V C</t>
         </is>
       </c>
-      <c r="L18" t="b">
-        <v>0</v>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>Federated States of Micronesia President David Panuelo warned the deal could stoke geopolitical tensions and undermine the sovereignty of the Pacific, while Samoa's Prime Minister, Fiame Naomi Mata'afa, suggested the process had been rushed. Pacific expert Anna Powles from Massey University told the ABC "very little" was currently known about the meeting but it seemed to be part of China's broader attempts to sideline the PIF. "It appears to be an attempt to deliberately disrupt existing regional mechanisms which China is not a part of," she said.</t>
-        </is>
+      <c r="K18" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1731,59 +1389,49 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Federated States of Micronesia President David Panuelo warned the deal could stoke geopolitical tensions and undermine the sovereignty of the Pacific, while Samoa's Prime Minister, Fiame Naomi Mata'afa, suggested the process had been rushed. Pacific expert Anna Powles from Massey University told the ABC "very little" was currently known about the meeting but it seemed to be part of China's broader attempts to sideline the PIF. "It appears to be an attempt to deliberately disrupt existing regional mechanisms which China is not a part of," she said.</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>the process had been rushed</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>the process had been rushed</t>
+          <t>(213, 240)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>(213, 240)</t>
+          <t>Samoa's Prime Minister, Fiame Naomi Mata'afa,</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Samoa's Prime Minister, Fiame Naomi Mata'afa,</t>
+          <t>(157, 202)</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>(157, 202)</t>
+          <t>suggested</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>suggested</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
           <t>(203, 212)</t>
         </is>
       </c>
-      <c r="J19" t="n">
+      <c r="I19" t="n">
         <v>5</v>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>S V C</t>
         </is>
       </c>
-      <c r="L19" t="b">
-        <v>0</v>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>Federated States of Micronesia President David Panuelo warned the deal could stoke geopolitical tensions and undermine the sovereignty of the Pacific, while Samoa's Prime Minister, Fiame Naomi Mata'afa, suggested the process had been rushed. Pacific expert Anna Powles from Massey University told the ABC "very little" was currently known about the meeting but it seemed to be part of China's broader attempts to sideline the PIF. "It appears to be an attempt to deliberately disrupt existing regional mechanisms which China is not a part of," she said.</t>
-        </is>
+      <c r="K19" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1794,59 +1442,49 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Federated States of Micronesia President David Panuelo warned the deal could stoke geopolitical tensions and undermine the sovereignty of the Pacific, while Samoa's Prime Minister, Fiame Naomi Mata'afa, suggested the process had been rushed. Pacific expert Anna Powles from Massey University told the ABC "very little" was currently known about the meeting but it seemed to be part of China's broader attempts to sideline the PIF. "It appears to be an attempt to deliberately disrupt existing regional mechanisms which China is not a part of," she said.</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>"very little" was currently known about the meeting</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>"very little" was currently known about the meeting</t>
+          <t>(305, 356)</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>(305, 356)</t>
+          <t>Pacific expert Anna Powles from Massey University</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Pacific expert Anna Powles from Massey University</t>
+          <t>(242, 291)</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>(242, 291)</t>
+          <t>told</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>told</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
           <t>(292, 296)</t>
         </is>
       </c>
-      <c r="J20" t="n">
+      <c r="I20" t="n">
         <v>10</v>
       </c>
-      <c r="K20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>S V C</t>
         </is>
       </c>
-      <c r="L20" t="b">
-        <v>0</v>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>Federated States of Micronesia President David Panuelo warned the deal could stoke geopolitical tensions and undermine the sovereignty of the Pacific, while Samoa's Prime Minister, Fiame Naomi Mata'afa, suggested the process had been rushed. Pacific expert Anna Powles from Massey University told the ABC "very little" was currently known about the meeting but it seemed to be part of China's broader attempts to sideline the PIF. "It appears to be an attempt to deliberately disrupt existing regional mechanisms which China is not a part of," she said.</t>
-        </is>
+      <c r="K20" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1857,59 +1495,49 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Federated States of Micronesia President David Panuelo warned the deal could stoke geopolitical tensions and undermine the sovereignty of the Pacific, while Samoa's Prime Minister, Fiame Naomi Mata'afa, suggested the process had been rushed. Pacific expert Anna Powles from Massey University told the ABC "very little" was currently known about the meeting but it seemed to be part of China's broader attempts to sideline the PIF. "It appears to be an attempt to deliberately disrupt existing regional mechanisms which China is not a part of," she said.</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>It appears to be an attempt to deliberately disrupt existing regional mechanisms which China is not a part of</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>It appears to be an attempt to deliberately disrupt existing regional mechanisms which China is not a part of</t>
+          <t>(432, 541)</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>(432, 541)</t>
+          <t>she</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>she</t>
+          <t>(544, 547)</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>(544, 547)</t>
+          <t>said</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>said</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
           <t>(548, 552)</t>
         </is>
       </c>
-      <c r="J21" t="n">
+      <c r="I21" t="n">
         <v>19</v>
       </c>
-      <c r="K21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>Q C Q S V</t>
         </is>
       </c>
-      <c r="L21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>Federated States of Micronesia President David Panuelo warned the deal could stoke geopolitical tensions and undermine the sovereignty of the Pacific, while Samoa's Prime Minister, Fiame Naomi Mata'afa, suggested the process had been rushed. Pacific expert Anna Powles from Massey University told the ABC "very little" was currently known about the meeting but it seemed to be part of China's broader attempts to sideline the PIF. "It appears to be an attempt to deliberately disrupt existing regional mechanisms which China is not a part of," she said.</t>
-        </is>
+      <c r="K21" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>